<commit_message>
feat: add detail jawaban page
</commit_message>
<xml_diff>
--- a/upload/temp/format_soal_download (1).xlsx
+++ b/upload/temp/format_soal_download (1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\namshin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\umbks\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>bobot</t>
   </si>
@@ -60,19 +60,94 @@
     <t>E</t>
   </si>
   <si>
-    <t>وَبُعُوْلَتُهُنَّ أَحَقُّ بِرَدِّهِنَّ فِي ذَالِكَ إنْ أرَادُوا إصْلاَحًا</t>
-  </si>
-  <si>
-    <t>مَثَلُ الّذِيْنَ يُنْفِقُونَ أمْوالَهُمْ فِي سَبِيْلِ الله كَمَثَلِ حَبَّةٍ أَنْبَتَتْ سَبْعَ سَنَابِلَ فِي كُلِّ سُنْبُلَةٍ مِائَةُ حَبَّةٍ  واللهُ يُضاعِفُ لِمَنْ يَشاء والله وَاسِعٌ عَلِيْمٌ</t>
-  </si>
-  <si>
-    <t>كُنْتُ نَهَيْتُكُمْ عَنْ زِيَارَةِ القُبُورِ فَزُوْرُوْهَا ( رواه مسلم )</t>
-  </si>
-  <si>
-    <t>وَلَا تَجْعَلْ يَدَكَ مَغْلُوْلَةً إلَى عُنُقِكَ وَلَا تَبْسُطْهَا كُلَّ الْبَسْطِ فَتَقْعُدَا مَلُوْمًا مَحْسُوْرًا</t>
-  </si>
-  <si>
-    <t xml:space="preserve">هَذا خَلْقُ اللهِ فَأرُونِي ماذا خَلَقَ الّذينَ مِنْ دُوْنِهِ بَلِ الظّالِمُون فِي ضَلَا لٍ مُبِيْن </t>
+    <t>Soal ke 1</t>
+  </si>
+  <si>
+    <t>Soal ke 2</t>
+  </si>
+  <si>
+    <t>Soal ke 3</t>
+  </si>
+  <si>
+    <t>Soal ke 4</t>
+  </si>
+  <si>
+    <t>Soal ke 5</t>
+  </si>
+  <si>
+    <t>opsi A.1</t>
+  </si>
+  <si>
+    <t>opsi A.2</t>
+  </si>
+  <si>
+    <t>opsi A.3</t>
+  </si>
+  <si>
+    <t>opsi A.4</t>
+  </si>
+  <si>
+    <t>opsi A.5</t>
+  </si>
+  <si>
+    <t>opsi B.1</t>
+  </si>
+  <si>
+    <t>opsi C.1</t>
+  </si>
+  <si>
+    <t>opsi D.1</t>
+  </si>
+  <si>
+    <t>opsi E.1</t>
+  </si>
+  <si>
+    <t>opsi B.2</t>
+  </si>
+  <si>
+    <t>opsi C.2</t>
+  </si>
+  <si>
+    <t>opsi D.2</t>
+  </si>
+  <si>
+    <t>opsi E.2</t>
+  </si>
+  <si>
+    <t>opsi B.3</t>
+  </si>
+  <si>
+    <t>opsi C.3</t>
+  </si>
+  <si>
+    <t>opsi D.3</t>
+  </si>
+  <si>
+    <t>opsi E.3</t>
+  </si>
+  <si>
+    <t>opsi B.4</t>
+  </si>
+  <si>
+    <t>opsi C.4</t>
+  </si>
+  <si>
+    <t>opsi D.4</t>
+  </si>
+  <si>
+    <t>opsi E.4</t>
+  </si>
+  <si>
+    <t>opsi B.5</t>
+  </si>
+  <si>
+    <t>opsi C.5</t>
+  </si>
+  <si>
+    <t>opsi D.5</t>
+  </si>
+  <si>
+    <t>opsi E.5</t>
   </si>
 </sst>
 </file>
@@ -124,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -134,9 +209,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,7 +519,7 @@
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7:G7"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -503,131 +575,131 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>14</v>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
       </c>
       <c r="H4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>15</v>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>16</v>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>17</v>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
       </c>
       <c r="H7" t="s">
         <v>8</v>

</xml_diff>